<commit_message>
working on oral presentation
</commit_message>
<xml_diff>
--- a/Chapters/drive_net/other/Tables.xlsx
+++ b/Chapters/drive_net/other/Tables.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1e993219bebc1327/PhD/Thesis/Overleaf Projects (8 items)/Drive-Net/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/personal-macbook/Documents/GitHubs/PhD/Draft/Chapters/drive_net/other/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="15" documentId="8_{9CB9710E-1143-C54B-9FF4-3AF7D42B7D3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2738B779-F122-964D-BC5F-61AC444A0825}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D4DE75B-BCC5-D94B-9A44-DFB742973D2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16340" activeTab="1" xr2:uid="{1047D54D-57FA-EA41-AC22-76EE7E48D314}"/>
   </bookViews>
@@ -191,7 +191,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
@@ -205,14 +205,13 @@
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -589,7 +588,7 @@
   <dimension ref="B3:C17"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B3" sqref="B3:C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -669,10 +668,10 @@
       </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="5"/>
+      <c r="C12" s="7"/>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B13" s="2" t="s">
@@ -699,7 +698,7 @@
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B17" s="7" t="s">
+      <c r="B17" t="s">
         <v>14</v>
       </c>
     </row>
@@ -718,7 +717,7 @@
   <dimension ref="B4:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B4" sqref="B4:E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -897,7 +896,7 @@
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="5" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>